<commit_message>
Se agrego tabla de riesgos a la matriz de riesgos con algunos riesgos
</commit_message>
<xml_diff>
--- a/Matriz_de_Riesgo.xlsx
+++ b/Matriz_de_Riesgo.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josro\OneDrive\Documentos\JORGE\SOFKA\TrainingQA\T2\2024-C1-QA-FP-T02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{868F2579-22EB-4588-9224-B8EC3A4F1FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71FE23A4-C4A9-4260-82E7-157ACC7DB7E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{17A1315E-0C82-45FD-941D-FBF90F3FEBDE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{17A1315E-0C82-45FD-941D-FBF90F3FEBDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="79">
   <si>
     <t>MATRIZ DE RIESGO</t>
   </si>
@@ -123,13 +124,163 @@
   </si>
   <si>
     <t>PROBABILIDAD</t>
+  </si>
+  <si>
+    <t>CODIGO DEL RIESGO</t>
+  </si>
+  <si>
+    <t>DESCRIPCION DEL RIESGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FASE AFECTADA</t>
+  </si>
+  <si>
+    <t>CAUSA RAIZ</t>
+  </si>
+  <si>
+    <t>ESTIMACION PROBABILIDAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESTIMACION IMPACTO </t>
+  </si>
+  <si>
+    <t>NIVEL DEL RIESGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESTRATEGIA A TOMAR </t>
+  </si>
+  <si>
+    <t>RESPONSIBLE DE ACCION</t>
+  </si>
+  <si>
+    <t>ID PROYECTO:</t>
+  </si>
+  <si>
+    <t>NOMBRE PROYECTO :</t>
+  </si>
+  <si>
+    <t>FECHA INICIAL:</t>
+  </si>
+  <si>
+    <t>FECHA FINAL:</t>
+  </si>
+  <si>
+    <t>RESPONSABLES MATRIZ:</t>
+  </si>
+  <si>
+    <t>2024-C1-QA-FP-T02</t>
+  </si>
+  <si>
+    <t>Taller T2 MERCADOLIBRE.COM.CO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOHAN CIFUENTES - JORGE RODRIGUEZ </t>
+  </si>
+  <si>
+    <t>TIPO DE RIESGO</t>
+  </si>
+  <si>
+    <t>PDT 001</t>
+  </si>
+  <si>
+    <t>PY 001</t>
+  </si>
+  <si>
+    <t>Requerimientos incompletos o ambiguos</t>
+  </si>
+  <si>
+    <t>Riesgo producto</t>
+  </si>
+  <si>
+    <t>Codificacion Sprint 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los requerimientos para el cambio del color del boton no se definieron de manera clara </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clarificar el codigo del color de boton </t>
+  </si>
+  <si>
+    <t>Product Owner</t>
+  </si>
+  <si>
+    <t>Licencia de Maternidad Desarrollador Fronted</t>
+  </si>
+  <si>
+    <t>Riesgo proyecto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El desarrollador de Fronted Yoreli Rincon tomara su licencia de maternidad </t>
+  </si>
+  <si>
+    <t>Equipo de desarrollo frontend</t>
+  </si>
+  <si>
+    <t>Codificacion Frontend Sprint 6</t>
+  </si>
+  <si>
+    <t>Codificacion Frontend futuras</t>
+  </si>
+  <si>
+    <t>5 Medio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reemplazar con un nuevo integrante al equipo de desarrollo front-end </t>
+  </si>
+  <si>
+    <t>Lider de Equipo</t>
+  </si>
+  <si>
+    <t>PDT 002</t>
+  </si>
+  <si>
+    <t>PDT 003</t>
+  </si>
+  <si>
+    <t>PDT 004</t>
+  </si>
+  <si>
+    <t>PDT 005</t>
+  </si>
+  <si>
+    <t>PY 002</t>
+  </si>
+  <si>
+    <t>PY 003</t>
+  </si>
+  <si>
+    <t>PY 004</t>
+  </si>
+  <si>
+    <t>PY 005</t>
+  </si>
+  <si>
+    <t>*Significado PDT= Riesgo en producto. PY= Riesgo en proyecto*</t>
+  </si>
+  <si>
+    <t>Incorporacion nuevo integrante de front-end</t>
+  </si>
+  <si>
+    <t>Riego de proyecto</t>
+  </si>
+  <si>
+    <t>Nuevo desarrrollador Front-end Junior, que iniciara en el proyecto</t>
+  </si>
+  <si>
+    <t>ENTREGABLE AFECTADO</t>
+  </si>
+  <si>
+    <t>Actualizarlo con el proyecto y capacitarlo con las tecnologias implementadas.</t>
+  </si>
+  <si>
+    <t>Desarrollador Senior</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,8 +288,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,6 +345,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -271,21 +450,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -298,14 +476,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -641,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC5AFB4-5F43-4353-B3E2-6A295DBC3CC1}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,34 +865,34 @@
     <col min="5" max="5" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="15" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-    </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-    </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="6"/>
       <c r="D4" s="1">
         <v>1</v>
       </c>
@@ -700,11 +909,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="5" t="s">
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -720,127 +929,127 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
       <c r="B6" s="1">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
       <c r="B7" s="1">
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
       <c r="B8" s="1">
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
       <c r="B9" s="1">
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="17" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="14" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B1:H1"/>
@@ -851,4 +1060,387 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49DE9FA9-E398-47DA-950D-69E8D4369C70}">
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="15"/>
+      <c r="C4" s="9">
+        <v>45362</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="9">
+        <v>45363</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="10">
+        <v>3</v>
+      </c>
+      <c r="H9" s="10">
+        <v>4</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="10">
+        <v>5</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+    </row>
+    <row r="15" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="10">
+        <v>3</v>
+      </c>
+      <c r="H15" s="10">
+        <v>3</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se finaliza la realizacion de la matriz de riesgo, queda pendiente de revision
</commit_message>
<xml_diff>
--- a/Matriz_de_Riesgo.xlsx
+++ b/Matriz_de_Riesgo.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josro\OneDrive\Documentos\JORGE\SOFKA\TrainingQA\T2\2024-C1-QA-FP-T02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71FE23A4-C4A9-4260-82E7-157ACC7DB7E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C183EF3-C10E-4429-9418-B89302432D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{17A1315E-0C82-45FD-941D-FBF90F3FEBDE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Grafico" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabala Riesgo" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="110">
   <si>
     <t>MATRIZ DE RIESGO</t>
   </si>
@@ -261,9 +261,6 @@
     <t>Incorporacion nuevo integrante de front-end</t>
   </si>
   <si>
-    <t>Riego de proyecto</t>
-  </si>
-  <si>
     <t>Nuevo desarrrollador Front-end Junior, que iniciara en el proyecto</t>
   </si>
   <si>
@@ -274,6 +271,102 @@
   </si>
   <si>
     <t>Desarrollador Senior</t>
+  </si>
+  <si>
+    <t>Accion</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Pendiente</t>
+  </si>
+  <si>
+    <t>Pruebas</t>
+  </si>
+  <si>
+    <t>El conjunto de pruebas realizadas no son suficientes para grarantizar el software esto sucede por omision y/o falta de tiempo.</t>
+  </si>
+  <si>
+    <t>Aseguramiento de calidad de software</t>
+  </si>
+  <si>
+    <t>No se realizan completitud de pruebas</t>
+  </si>
+  <si>
+    <t>Capacitacion superficial a ususarios finales</t>
+  </si>
+  <si>
+    <t>Entrega del producto</t>
+  </si>
+  <si>
+    <t>Por limitacion de tiempo se realizan capacitaciones incompletas sobre el uso de la aplicacion</t>
+  </si>
+  <si>
+    <t>Produccion entregable</t>
+  </si>
+  <si>
+    <t>Se sugiere dar un seguimiento a la capacitacion faltante o incompleta</t>
+  </si>
+  <si>
+    <t>Se muestra una limitacion a usuarios de 18 años para productos</t>
+  </si>
+  <si>
+    <t>Los limites para que los ususarios de 18 años puedan ingresar para hacer comprar por omision del signo en el codigo &gt;=</t>
+  </si>
+  <si>
+    <t>Codificacion Backend</t>
+  </si>
+  <si>
+    <t>Se sugiere arreglar el error</t>
+  </si>
+  <si>
+    <t>Equipo Backend</t>
+  </si>
+  <si>
+    <t>Subestimacion del tamaño de la aplicación</t>
+  </si>
+  <si>
+    <t>Diseño</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Al realizar el diseño se subestimo el software con respecto a las necesidades del cliente </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diseño </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fallas del hadware limitan la funcionalidad del software </t>
+  </si>
+  <si>
+    <t>La intensidad de la red, hace una caida o demora en la carga de algunos servicios</t>
+  </si>
+  <si>
+    <t>Nuevos requerimientos a la funcion de crear usuario</t>
+  </si>
+  <si>
+    <t>El nuevo requerimiento de añadir preposiciones que los clientes desean en sus usuarios puede causar ambigüedad</t>
+  </si>
+  <si>
+    <t>Celula de desarrollo</t>
+  </si>
+  <si>
+    <t>Conflicto por versiones de Java en Desarrolladores Backend</t>
+  </si>
+  <si>
+    <t>Equipo de desarrollo Backend</t>
+  </si>
+  <si>
+    <t>Conflicto por diferentes versiones de Java 11 y Java 17</t>
+  </si>
+  <si>
+    <t>Resuelto</t>
+  </si>
+  <si>
+    <t>Realizazon la sincronizacion de todo el equipo con Java 17</t>
+  </si>
+  <si>
+    <t>*Los riesgos que se encuentran vacios, estan en espera a respuesta del responsible*</t>
   </si>
 </sst>
 </file>
@@ -450,32 +543,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -489,32 +561,57 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -853,7 +950,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,33 +963,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="18"/>
       <c r="D4" s="1">
         <v>1</v>
       </c>
@@ -910,9 +1007,9 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
@@ -930,122 +1027,122 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="1">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="20" t="s">
+      <c r="H6" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="1">
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="11" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="1">
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="1">
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="8" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1064,10 +1161,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49DE9FA9-E398-47DA-950D-69E8D4369C70}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,361 +1182,501 @@
     <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="15"/>
+      <c r="B2" s="22"/>
       <c r="C2" t="s">
         <v>43</v>
       </c>
-      <c r="J2" t="s">
+      <c r="H2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="15"/>
+      <c r="B3" s="22"/>
       <c r="C3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="H3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="9">
+      <c r="B4" s="22"/>
+      <c r="C4" s="2">
         <v>45362</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="9">
+      <c r="B5" s="22"/>
+      <c r="C5" s="2">
         <v>45363</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="15"/>
+      <c r="B6" s="22"/>
       <c r="C6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+    <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="3">
+        <v>3</v>
+      </c>
+      <c r="H9" s="3">
+        <v>4</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="L9" s="23"/>
+      <c r="M9" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="3">
+        <v>3</v>
+      </c>
+      <c r="H10" s="3">
+        <v>5</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="L10" s="23"/>
+      <c r="M10" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G11" s="3">
+        <v>2</v>
+      </c>
+      <c r="H11" s="3">
+        <v>5</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="L11" s="23"/>
+      <c r="M11" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3">
+        <v>3</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="L12" s="23"/>
+      <c r="M12" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" s="3">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3">
+        <v>2</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="L13" s="23"/>
+      <c r="M13" s="24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1</v>
+      </c>
+      <c r="H14" s="3">
+        <v>5</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L14" s="23"/>
+      <c r="M14" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="3">
+        <v>3</v>
+      </c>
+      <c r="H15" s="3">
+        <v>3</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="G8" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="K8" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" s="10">
+      <c r="K15" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="L15" s="23"/>
+      <c r="M15" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" s="3">
         <v>3</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H16" s="3">
         <v>4</v>
       </c>
-      <c r="I9" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="K9" s="10" t="s">
+      <c r="I16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K16" s="3"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3">
+        <v>4</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="10" t="s">
+      <c r="L17" s="23"/>
+      <c r="M17" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G10" s="10">
-        <v>1</v>
-      </c>
-      <c r="H10" s="10">
-        <v>5</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="K10" s="10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-    </row>
-    <row r="15" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="10">
-        <v>3</v>
-      </c>
-      <c r="H15" s="10">
-        <v>3</v>
-      </c>
-      <c r="I15" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="J15" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="K15" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
+      <c r="D18" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G18" s="3">
+        <v>4</v>
+      </c>
+      <c r="H18" s="3">
+        <v>4</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="L18" s="23"/>
+      <c r="M18" s="24" t="s">
+        <v>80</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>